<commit_message>
PC-Template and corresponding Xcel ready for coding
</commit_message>
<xml_diff>
--- a/AXA/Book1(1).xlsx
+++ b/AXA/Book1(1).xlsx
@@ -13,13 +13,14 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="91">
   <si>
     <t>Removal for processing Remarks</t>
   </si>
@@ -108,90 +109,96 @@
     <t>Place</t>
   </si>
   <si>
-    <t>Range And Division Address</t>
-  </si>
-  <si>
-    <t>File Name</t>
+    <t>RangeAndDivisionAddress</t>
+  </si>
+  <si>
+    <t>FileName</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>B-17 Bond Amount</t>
-  </si>
-  <si>
-    <t>Bank Guarantee</t>
-  </si>
-  <si>
-    <t>B.G. dt.</t>
-  </si>
-  <si>
-    <t>B. G. Amount</t>
-  </si>
-  <si>
-    <t>B. G. Valid Dt.</t>
-  </si>
-  <si>
-    <t>Division Address</t>
-  </si>
-  <si>
-    <t>B-17 Bond entry no.</t>
-  </si>
-  <si>
-    <t>B-17 Bond entry dt.</t>
-  </si>
-  <si>
-    <t>IC No.</t>
-  </si>
-  <si>
-    <t>IC Date</t>
-  </si>
-  <si>
-    <t>Chapter No.</t>
-  </si>
-  <si>
-    <t>CTH No.</t>
-  </si>
-  <si>
-    <t>Name of Supplier</t>
-  </si>
-  <si>
-    <t>County Name</t>
-  </si>
-  <si>
-    <t>Description of goods</t>
+    <t>B-17BondAmount</t>
+  </si>
+  <si>
+    <t>BankGuaranteeNo</t>
+  </si>
+  <si>
+    <t>BGDate</t>
+  </si>
+  <si>
+    <t>BGAmount</t>
+  </si>
+  <si>
+    <t>BGValidDate</t>
+  </si>
+  <si>
+    <t>DivisionAddress</t>
+  </si>
+  <si>
+    <t>B-17BondEntryNo</t>
+  </si>
+  <si>
+    <t>B-17BondEntryDate</t>
+  </si>
+  <si>
+    <t>ICNumber</t>
+  </si>
+  <si>
+    <t>ICDate</t>
+  </si>
+  <si>
+    <t>ProformaInvoiceNo</t>
+  </si>
+  <si>
+    <t>ProformaInvoiceDate</t>
+  </si>
+  <si>
+    <t>ChapterNo</t>
+  </si>
+  <si>
+    <t>CTHNo</t>
+  </si>
+  <si>
+    <t>DescriptionofGoods</t>
   </si>
   <si>
     <t>Qty</t>
   </si>
   <si>
+    <t>GrandTotal</t>
+  </si>
+  <si>
+    <t>B-17Bond25percentDebit</t>
+  </si>
+  <si>
+    <t>RunningB-17BondBalance</t>
+  </si>
+  <si>
+    <t>Form A</t>
+  </si>
+  <si>
+    <t>Bond No.</t>
+  </si>
+  <si>
+    <t>Bill of Entry No. and date, if applicable</t>
+  </si>
+  <si>
+    <t>Customs Station of import, if applicable</t>
+  </si>
+  <si>
+    <t>Code and address of Warehouse from where received (only in cases goods are procured from public or private warehouse)</t>
+  </si>
+  <si>
+    <t>Client Name And  address</t>
+  </si>
+  <si>
+    <t>Others (in case of any other source of procurement)</t>
+  </si>
+  <si>
     <t>B-17 Bond 25% Debit</t>
   </si>
   <si>
-    <t>Running B-17 Bond  Balance</t>
-  </si>
-  <si>
-    <t>Form A</t>
-  </si>
-  <si>
-    <t>Bond No.</t>
-  </si>
-  <si>
-    <t>Bill of Entry No. and date, if applicable</t>
-  </si>
-  <si>
-    <t>Customs Station of import, if applicable</t>
-  </si>
-  <si>
-    <t>Code and address of Warehouse from where received (only in cases goods are procured from public or private warehouse)</t>
-  </si>
-  <si>
-    <t>Client Name And  address</t>
-  </si>
-  <si>
-    <t>Others (in case of any other source of procurement)</t>
-  </si>
-  <si>
     <t>Broad Description</t>
   </si>
   <si>
@@ -280,9 +287,6 @@
   </si>
   <si>
     <t>123,5</t>
-  </si>
-  <si>
-    <t>ClientContactPersonNameEmailAnd  &lt; ContactNo</t>
   </si>
   <si>
     <t>123,6</t>
@@ -298,7 +302,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -322,6 +326,12 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibiri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -330,12 +340,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -392,7 +408,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -401,7 +417,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,7 +433,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -417,7 +441,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -430,6 +458,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -440,8 +528,8 @@
   </sheetPr>
   <dimension ref="A1:CE5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T5" activeCellId="0" sqref="T5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AW1" activeCellId="0" sqref="AW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -451,7 +539,9 @@
     <col collapsed="false" hidden="false" max="9" min="4" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="17" min="10" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.57085020242915"/>
-    <col collapsed="false" hidden="false" max="59" min="19" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="46" min="19" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="2" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="59" min="48" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="60" min="60" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="67" min="61" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="68" min="68" style="1" width="19.5748987854251"/>
@@ -483,320 +573,322 @@
       <c r="U1" s="0"/>
       <c r="V1" s="0"/>
       <c r="W1" s="0"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-      <c r="BD1" s="2"/>
-      <c r="BE1" s="2"/>
-      <c r="BF1" s="2"/>
-      <c r="BG1" s="2"/>
-      <c r="BH1" s="2"/>
-      <c r="BI1" s="2"/>
-      <c r="BJ1" s="2"/>
-      <c r="BK1" s="2"/>
-      <c r="BL1" s="3" t="s">
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="3"/>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="4"/>
+      <c r="AV1" s="3"/>
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3"/>
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
+      <c r="BI1" s="3"/>
+      <c r="BJ1" s="3"/>
+      <c r="BK1" s="3"/>
+      <c r="BL1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="BM1" s="3"/>
-      <c r="BN1" s="3"/>
-      <c r="BO1" s="3"/>
-      <c r="BP1" s="3" t="s">
+      <c r="BM1" s="5"/>
+      <c r="BN1" s="5"/>
+      <c r="BO1" s="5"/>
+      <c r="BP1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BQ1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="BR1" s="3"/>
-      <c r="BS1" s="3"/>
-      <c r="BT1" s="3"/>
-      <c r="BU1" s="3"/>
-      <c r="BV1" s="3"/>
-      <c r="BW1" s="3" t="s">
+      <c r="BR1" s="5"/>
+      <c r="BS1" s="5"/>
+      <c r="BT1" s="5"/>
+      <c r="BU1" s="5"/>
+      <c r="BV1" s="5"/>
+      <c r="BW1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BX1" s="3"/>
-      <c r="BY1" s="3"/>
-      <c r="BZ1" s="3"/>
-      <c r="CA1" s="3"/>
-      <c r="CB1" s="3"/>
-      <c r="CC1" s="3" t="s">
+      <c r="BX1" s="5"/>
+      <c r="BY1" s="5"/>
+      <c r="BZ1" s="5"/>
+      <c r="CA1" s="5"/>
+      <c r="CB1" s="5"/>
+      <c r="CC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="CD1" s="3"/>
-      <c r="CE1" s="3"/>
+      <c r="CD1" s="5"/>
+      <c r="CE1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2" t="s">
+      <c r="Y2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="Z2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AA2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AB2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AC2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AD2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AE2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AF2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AG2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AH2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AI2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AK2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AL2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AM2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AN2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AO2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AP2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AR2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AS2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AU2" s="2"/>
-      <c r="AV2" s="6" t="s">
+      <c r="AT2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AW2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="AX2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="AY2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="BB2" s="2" t="s">
+      <c r="BA2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BC2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BB2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BC2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="BF2" s="2" t="s">
+      <c r="BD2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BE2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="BH2" s="2" t="s">
+      <c r="BF2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="BI2" s="2" t="s">
+      <c r="BG2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="BJ2" s="2" t="s">
+      <c r="BH2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="BK2" s="2" t="s">
+      <c r="BI2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="BL2" s="2" t="s">
+      <c r="BJ2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="BM2" s="2" t="s">
+      <c r="BK2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="BN2" s="2" t="s">
+      <c r="BL2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="BO2" s="2" t="s">
+      <c r="BM2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="BP2" s="3"/>
-      <c r="BQ2" s="2" t="s">
+      <c r="BN2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="BR2" s="2" t="s">
+      <c r="BO2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="BS2" s="2" t="s">
+      <c r="BP2" s="5"/>
+      <c r="BQ2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="BT2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BU2" s="2" t="s">
+      <c r="BR2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="BV2" s="2" t="s">
+      <c r="BS2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="BW2" s="2" t="s">
+      <c r="BT2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="BX2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BY2" s="2" t="s">
+      <c r="BU2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="BV2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BW2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="BZ2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="CA2" s="2" t="s">
+      <c r="BX2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="CB2" s="2" t="s">
+      <c r="BY2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="CC2" s="2" t="s">
+      <c r="BZ2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="CA2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="CD2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="CE2" s="2" t="s">
+      <c r="CB2" s="3" t="s">
         <v>75</v>
+      </c>
+      <c r="CC2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="CD2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="CE2" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,79 +896,79 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="U3" s="3" t="s">
+      <c r="T3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="X3" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="AP3" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="AQ3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR3" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,79 +976,79 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="U4" s="3" t="s">
+      <c r="T4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="AP4" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="AQ4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR4" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,79 +1056,79 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="U5" s="3" t="s">
+      <c r="T5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="U5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="V5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="W5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="X5" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="AP5" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="AQ5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR5" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PC and column names configurable
</commit_message>
<xml_diff>
--- a/AXA/Book1(1).xlsx
+++ b/AXA/Book1(1).xlsx
@@ -14,13 +14,14 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
   <si>
     <t>Removal for processing Remarks</t>
   </si>
@@ -118,55 +119,178 @@
     <t>Date</t>
   </si>
   <si>
+    <t>B17BondAmount</t>
+  </si>
+  <si>
+    <t>BankGuaranteeNo</t>
+  </si>
+  <si>
+    <t>BGDate</t>
+  </si>
+  <si>
+    <t>BGAmount</t>
+  </si>
+  <si>
+    <t>BGValidDate</t>
+  </si>
+  <si>
+    <t>DivisionAddress</t>
+  </si>
+  <si>
+    <t>B17BondEntryNo</t>
+  </si>
+  <si>
+    <t>B17BondEntryDate</t>
+  </si>
+  <si>
+    <t>ICNumber</t>
+  </si>
+  <si>
+    <t>ICDate</t>
+  </si>
+  <si>
+    <t>ProformaInvoiceNo</t>
+  </si>
+  <si>
+    <t>ProformaInvoiceDate</t>
+  </si>
+  <si>
+    <t>ChapterNo</t>
+  </si>
+  <si>
+    <t>CTHNo</t>
+  </si>
+  <si>
+    <t>DescriptionofGoods</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>GrandTotal</t>
+  </si>
+  <si>
+    <t>B17Bond25percentDebit</t>
+  </si>
+  <si>
+    <t>RunningB17BondBalance</t>
+  </si>
+  <si>
+    <t>Form A</t>
+  </si>
+  <si>
+    <t>Bond No.</t>
+  </si>
+  <si>
+    <t>Bill of Entry No. and date, if applicable</t>
+  </si>
+  <si>
+    <t>Customs Station of import, if applicable</t>
+  </si>
+  <si>
+    <t>Code and address of Warehouse from where received (only in cases goods are procured from public or private warehouse)</t>
+  </si>
+  <si>
+    <t>Client Name And  address</t>
+  </si>
+  <si>
+    <t>Others (in case of any other source of procurement)</t>
+  </si>
+  <si>
+    <t>B-17 Bond 25% Debit</t>
+  </si>
+  <si>
+    <t>Broad Description</t>
+  </si>
+  <si>
+    <t>Invoice No. And  Dt.</t>
+  </si>
+  <si>
+    <t>Procurement Certificate No. and date</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>Assessable Value</t>
+  </si>
+  <si>
+    <t>Duty assessed</t>
+  </si>
+  <si>
+    <t>Registration No. of means of transport</t>
+  </si>
+  <si>
+    <t>Date and time of receipt</t>
+  </si>
+  <si>
+    <t>Date and time of removal</t>
+  </si>
+  <si>
+    <t>Quantity cleared</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Duty involved</t>
+  </si>
+  <si>
+    <t>Purpose of removal</t>
+  </si>
+  <si>
+    <t>Date and Time</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Duty</t>
+  </si>
+  <si>
+    <t>Details of document under which removed (No. and date)</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Northern Operating Services Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>SubBranch1</t>
+  </si>
+  <si>
+    <t>Floor 1, Tower D, Tech Park One, Survey No.191, Hissa No.2A/1/2, City Survey No.2175 Village Yerwada, Airport Road, Yerwada,  Pune - 411006</t>
+  </si>
+  <si>
+    <t>123,4</t>
+  </si>
+  <si>
+    <t>ExtensionofLOPNoAnd Date</t>
+  </si>
+  <si>
+    <t>CustomBondingLicenseNoAnd Date</t>
+  </si>
+  <si>
+    <t>InvoiceNoAnd Date</t>
+  </si>
+  <si>
+    <t>ClientContactPersonNameEmailAnd ContactNo</t>
+  </si>
+  <si>
     <t>B-17BondAmount</t>
   </si>
   <si>
-    <t>BankGuaranteeNo</t>
-  </si>
-  <si>
-    <t>BGDate</t>
-  </si>
-  <si>
-    <t>BGAmount</t>
-  </si>
-  <si>
-    <t>BGValidDate</t>
-  </si>
-  <si>
-    <t>DivisionAddress</t>
-  </si>
-  <si>
     <t>B-17BondEntryNo</t>
   </si>
   <si>
     <t>B-17BondEntryDate</t>
   </si>
   <si>
-    <t>ICNumber</t>
-  </si>
-  <si>
-    <t>ICDate</t>
-  </si>
-  <si>
-    <t>ProformaInvoiceNo</t>
-  </si>
-  <si>
-    <t>ProformaInvoiceDate</t>
-  </si>
-  <si>
-    <t>ChapterNo</t>
-  </si>
-  <si>
-    <t>CTHNo</t>
-  </si>
-  <si>
-    <t>DescriptionofGoods</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>GrandTotal</t>
+    <t>1. Description^p2. ofGoodss</t>
   </si>
   <si>
     <t>B-17Bond25percentDebit</t>
@@ -175,118 +299,13 @@
     <t>RunningB-17BondBalance</t>
   </si>
   <si>
-    <t>Form A</t>
-  </si>
-  <si>
-    <t>Bond No.</t>
-  </si>
-  <si>
-    <t>Bill of Entry No. and date, if applicable</t>
-  </si>
-  <si>
-    <t>Customs Station of import, if applicable</t>
-  </si>
-  <si>
-    <t>Code and address of Warehouse from where received (only in cases goods are procured from public or private warehouse)</t>
-  </si>
-  <si>
-    <t>Client Name And  address</t>
-  </si>
-  <si>
-    <t>Others (in case of any other source of procurement)</t>
-  </si>
-  <si>
-    <t>B-17 Bond 25% Debit</t>
-  </si>
-  <si>
-    <t>Broad Description</t>
-  </si>
-  <si>
-    <t>Invoice No. And  Dt.</t>
-  </si>
-  <si>
-    <t>Procurement Certificate No. and date</t>
-  </si>
-  <si>
-    <t>QTY</t>
-  </si>
-  <si>
-    <t>Assessable Value</t>
-  </si>
-  <si>
-    <t>Duty assessed</t>
-  </si>
-  <si>
-    <t>Registration No. of means of transport</t>
-  </si>
-  <si>
-    <t>Date and time of receipt</t>
-  </si>
-  <si>
-    <t>Date and time of removal</t>
-  </si>
-  <si>
-    <t>Quantity cleared</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Duty involved</t>
-  </si>
-  <si>
-    <t>Purpose of removal</t>
-  </si>
-  <si>
-    <t>Date and Time</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>Duty</t>
-  </si>
-  <si>
-    <t>Details of document under which removed (No. and date)</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Northern Operating Services Pvt. Ltd.</t>
-  </si>
-  <si>
-    <t>SubBranch1</t>
-  </si>
-  <si>
-    <t>Floor 1, Tower D, Tech Park One, Survey No.191, Hissa No.2A/1/2, City Survey No.2175 Village Yerwada, Airport Road, Yerwada,  Pune - 411006</t>
-  </si>
-  <si>
-    <t>123,4</t>
-  </si>
-  <si>
-    <t>ExtensionofLOPNoAnd Date</t>
-  </si>
-  <si>
-    <t>CustomBondingLicenseNoAnd Date</t>
-  </si>
-  <si>
-    <t>InvoiceNoAnd Date</t>
-  </si>
-  <si>
-    <t>ClientContactPersonNameEmailAnd ContactNo</t>
+    <t>SubBranch3</t>
+  </si>
+  <si>
+    <t>123,5</t>
   </si>
   <si>
     <t>1. 2.</t>
-  </si>
-  <si>
-    <t>SubBranch3</t>
-  </si>
-  <si>
-    <t>123,5</t>
   </si>
   <si>
     <t>123,6</t>
@@ -408,16 +427,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -528,8 +543,8 @@
   </sheetPr>
   <dimension ref="A1:CE5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AP3" activeCellId="0" sqref="AP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -539,9 +554,7 @@
     <col collapsed="false" hidden="false" max="9" min="4" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="17" min="10" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.57085020242915"/>
-    <col collapsed="false" hidden="false" max="46" min="19" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="2" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="59" min="48" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="59" min="19" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="60" min="60" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="67" min="61" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="68" min="68" style="1" width="19.5748987854251"/>
@@ -573,321 +586,321 @@
       <c r="U1" s="0"/>
       <c r="V1" s="0"/>
       <c r="W1" s="0"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="4"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3"/>
-      <c r="BA1" s="3"/>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3"/>
-      <c r="BD1" s="3"/>
-      <c r="BE1" s="3"/>
-      <c r="BF1" s="3"/>
-      <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
-      <c r="BI1" s="3"/>
-      <c r="BJ1" s="3"/>
-      <c r="BK1" s="3"/>
-      <c r="BL1" s="5" t="s">
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BM1" s="5"/>
-      <c r="BN1" s="5"/>
-      <c r="BO1" s="5"/>
-      <c r="BP1" s="5" t="s">
+      <c r="BM1" s="4"/>
+      <c r="BN1" s="4"/>
+      <c r="BO1" s="4"/>
+      <c r="BP1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="BR1" s="5"/>
-      <c r="BS1" s="5"/>
-      <c r="BT1" s="5"/>
-      <c r="BU1" s="5"/>
-      <c r="BV1" s="5"/>
-      <c r="BW1" s="5" t="s">
+      <c r="BR1" s="4"/>
+      <c r="BS1" s="4"/>
+      <c r="BT1" s="4"/>
+      <c r="BU1" s="4"/>
+      <c r="BV1" s="4"/>
+      <c r="BW1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="BX1" s="5"/>
-      <c r="BY1" s="5"/>
-      <c r="BZ1" s="5"/>
-      <c r="CA1" s="5"/>
-      <c r="CB1" s="5"/>
-      <c r="CC1" s="5" t="s">
+      <c r="BX1" s="4"/>
+      <c r="BY1" s="4"/>
+      <c r="BZ1" s="4"/>
+      <c r="CA1" s="4"/>
+      <c r="CB1" s="4"/>
+      <c r="CC1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="CD1" s="5"/>
-      <c r="CE1" s="5"/>
+      <c r="CD1" s="4"/>
+      <c r="CE1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AL2" s="8" t="s">
+      <c r="AL2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AM2" s="8" t="s">
+      <c r="AM2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AN2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AO2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AP2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AR2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AS2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AT2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AU2" s="4"/>
-      <c r="AV2" s="9" t="s">
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AW2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AX2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="AY2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BA2" s="6" t="s">
+      <c r="BA2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BB2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BC2" s="6" t="s">
+      <c r="BC2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="BD2" s="6" t="s">
+      <c r="BD2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="BE2" s="6" t="s">
+      <c r="BE2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BF2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BG2" s="6" t="s">
+      <c r="BG2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BH2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BI2" s="3" t="s">
+      <c r="BI2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BJ2" s="3" t="s">
+      <c r="BJ2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BK2" s="3" t="s">
+      <c r="BK2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BL2" s="3" t="s">
+      <c r="BL2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BM2" s="3" t="s">
+      <c r="BM2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BN2" s="3" t="s">
+      <c r="BN2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BO2" s="3" t="s">
+      <c r="BO2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BP2" s="5"/>
-      <c r="BQ2" s="3" t="s">
+      <c r="BP2" s="4"/>
+      <c r="BQ2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BR2" s="3" t="s">
+      <c r="BR2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BS2" s="3" t="s">
+      <c r="BS2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BT2" s="3" t="s">
+      <c r="BT2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BU2" s="3" t="s">
+      <c r="BU2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BV2" s="3" t="s">
+      <c r="BV2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BW2" s="3" t="s">
+      <c r="BW2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BX2" s="3" t="s">
+      <c r="BX2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BY2" s="3" t="s">
+      <c r="BY2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BZ2" s="3" t="s">
+      <c r="BZ2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="CA2" s="3" t="s">
+      <c r="CA2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="CB2" s="3" t="s">
+      <c r="CB2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="CC2" s="3" t="s">
+      <c r="CC2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="CD2" s="3" t="s">
+      <c r="CD2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="CE2" s="3" t="s">
+      <c r="CE2" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -925,50 +938,110 @@
       <c r="K3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="W3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="Y3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AQ3" s="1" t="s">
-        <v>86</v>
+      <c r="AC3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,13 +1052,13 @@
         <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -1005,50 +1078,50 @@
       <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="S4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="7" t="s">
+      <c r="W4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="X4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="AQ4" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1059,13 +1132,13 @@
         <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -1085,50 +1158,50 @@
       <c r="K5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="U5" s="5" t="s">
+      <c r="T5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="V5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="W5" s="7" t="s">
+      <c r="W5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="X5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed table lines and handled file open exception
</commit_message>
<xml_diff>
--- a/AXA/Book1(1).xlsx
+++ b/AXA/Book1(1).xlsx
@@ -1,27 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Sheet1!$AT$1:$AT$1048575</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$AT$1:$AT$1048575</definedName>
+    <definedName name="Print_Area_0" localSheetId="0">Sheet1!$AT$1:$AT$1048575</definedName>
+    <definedName name="Print_Area_0_0" localSheetId="0">Sheet1!$AT$1:$AT$1048575</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="104">
   <si>
     <t>Removal for processing Remarks</t>
   </si>
@@ -290,9 +288,6 @@
     <t>B-17BondEntryDate</t>
   </si>
   <si>
-    <t>1. Description^p2. ofGoodss</t>
-  </si>
-  <si>
     <t>B-17Bond25percentDebit</t>
   </si>
   <si>
@@ -312,16 +307,37 @@
   </si>
   <si>
     <t>ClientContactPersonNameEmail &amp;amp;  ContactNo</t>
+  </si>
+  <si>
+    <t>NewUsedEquipment 1</t>
+  </si>
+  <si>
+    <t>NNN</t>
+  </si>
+  <si>
+    <t>NewUsedEquipment 313 !@#$%^&amp;*()_+</t>
+  </si>
+  <si>
+    <t>1. Description^p 2. ofGoodss</t>
+  </si>
+  <si>
+    <t>1. 1 2. 5</t>
+  </si>
+  <si>
+    <t>1. 22 2. 33</t>
+  </si>
+  <si>
+    <t>1. 100 2. 200</t>
+  </si>
+  <si>
+    <t>cthno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -330,28 +346,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibiri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -380,99 +380,83 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -531,61 +515,349 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:CE5"/>
+  <dimension ref="A1:AMI5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP3" activeCellId="0" sqref="AP3"/>
+    <sheetView tabSelected="1" topLeftCell="Z3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="11.7125506072874"/>
-    <col collapsed="false" hidden="false" max="9" min="4" style="1" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="17" min="10" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="9.57085020242915"/>
-    <col collapsed="false" hidden="false" max="59" min="19" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="67" min="61" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="1" width="19.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1023" min="69" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.1417004048583"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="3" width="11.7265625" style="1"/>
+    <col min="4" max="9" width="14.1796875" style="1"/>
+    <col min="10" max="17" width="9.1796875" style="1"/>
+    <col min="18" max="18" width="9.54296875" style="1"/>
+    <col min="19" max="59" width="9.1796875" style="1"/>
+    <col min="60" max="60" width="10.7265625" style="1"/>
+    <col min="61" max="67" width="9.1796875" style="1"/>
+    <col min="68" max="68" width="19.54296875" style="1"/>
+    <col min="69" max="1023" width="9.1796875" style="1"/>
+    <col min="1024" max="1025" width="9.1796875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="L1" s="0"/>
-      <c r="M1" s="0"/>
-      <c r="N1" s="0"/>
-      <c r="O1" s="0"/>
-      <c r="P1" s="0"/>
-      <c r="Q1" s="0"/>
-      <c r="R1" s="0"/>
-      <c r="S1" s="0"/>
-      <c r="T1" s="0"/>
-      <c r="U1" s="0"/>
-      <c r="V1" s="0"/>
-      <c r="W1" s="0"/>
+    <row r="1" spans="1:83" ht="62.25" customHeight="1">
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
@@ -626,38 +898,38 @@
       <c r="BI1" s="2"/>
       <c r="BJ1" s="2"/>
       <c r="BK1" s="2"/>
-      <c r="BL1" s="4" t="s">
+      <c r="BL1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="BM1" s="4"/>
-      <c r="BN1" s="4"/>
-      <c r="BO1" s="4"/>
-      <c r="BP1" s="4" t="s">
+      <c r="BM1" s="9"/>
+      <c r="BN1" s="9"/>
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BQ1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="BR1" s="4"/>
-      <c r="BS1" s="4"/>
-      <c r="BT1" s="4"/>
-      <c r="BU1" s="4"/>
-      <c r="BV1" s="4"/>
-      <c r="BW1" s="4" t="s">
+      <c r="BR1" s="9"/>
+      <c r="BS1" s="9"/>
+      <c r="BT1" s="9"/>
+      <c r="BU1" s="9"/>
+      <c r="BV1" s="9"/>
+      <c r="BW1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="BX1" s="4"/>
-      <c r="BY1" s="4"/>
-      <c r="BZ1" s="4"/>
-      <c r="CA1" s="4"/>
-      <c r="CB1" s="4"/>
-      <c r="CC1" s="4" t="s">
+      <c r="BX1" s="9"/>
+      <c r="BY1" s="9"/>
+      <c r="BZ1" s="9"/>
+      <c r="CA1" s="9"/>
+      <c r="CB1" s="9"/>
+      <c r="CC1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="CD1" s="4"/>
-      <c r="CE1" s="4"/>
+      <c r="CD1" s="9"/>
+      <c r="CE1" s="9"/>
     </row>
-    <row r="2" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:83" ht="232">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -857,7 +1129,7 @@
       <c r="BO2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BP2" s="4"/>
+      <c r="BP2" s="9"/>
       <c r="BQ2" s="2" t="s">
         <v>71</v>
       </c>
@@ -904,8 +1176,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:83" ht="159.5">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -942,7 +1214,7 @@
         <v>16</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>18</v>
@@ -956,8 +1228,8 @@
       <c r="Q3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>22</v>
+      <c r="R3" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>23</v>
@@ -1025,40 +1297,40 @@
       <c r="AN3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AO3" s="5" t="s">
-        <v>45</v>
+      <c r="AO3" s="10" t="s">
+        <v>101</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="AR3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="AS3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AT3" s="2" t="s">
-        <v>91</v>
-      </c>
     </row>
-    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:83" ht="159.5">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -1082,7 +1354,7 @@
         <v>16</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>18</v>
@@ -1117,28 +1389,31 @@
       <c r="X4" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="AO4" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="AP4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AQ4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:83" ht="159.5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -1162,7 +1437,7 @@
         <v>16</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>18</v>
@@ -1183,7 +1458,7 @@
         <v>23</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U5" s="4" t="s">
         <v>25</v>
@@ -1198,10 +1473,10 @@
         <v>28</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1212,12 +1487,7 @@
     <mergeCell ref="BW1:CB1"/>
     <mergeCell ref="CC1:CE1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>